<commit_message>
EST-1861: adds term sheet
</commit_message>
<xml_diff>
--- a/estatioapp/app/src/test/java/org/estatio/module/capex/integtests/project/Projects OXF.xlsx
+++ b/estatioapp/app/src/test/java/org/estatio/module/capex/integtests/project/Projects OXF.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="33460" windowHeight="17900"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="33460" windowHeight="17900" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="projects" sheetId="1" r:id="rId1"/>
+    <sheet name="terms" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -592,7 +593,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="G4" sqref="G4"/>
     </sheetView>
@@ -754,4 +755,21 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
EST-1860: adds terms to project import integration test
</commit_message>
<xml_diff>
--- a/estatioapp/app/src/test/java/org/estatio/module/capex/integtests/project/Projects OXF.xlsx
+++ b/estatioapp/app/src/test/java/org/estatio/module/capex/integtests/project/Projects OXF.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="28">
   <si>
     <t>Project Reference</t>
   </si>
@@ -101,6 +101,9 @@
   </si>
   <si>
     <t>some works</t>
+  </si>
+  <si>
+    <t>budgetedAmount</t>
   </si>
 </sst>
 </file>
@@ -159,9 +162,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="48">
+  <cellStyleXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -214,7 +229,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="48">
+  <cellStyles count="60">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
@@ -239,6 +254,12 @@
     <cellStyle name="Followed Hyperlink" xfId="43" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="45" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="47" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="49" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="51" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="53" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="55" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="57" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="59" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -262,6 +283,12 @@
     <cellStyle name="Hyperlink" xfId="42" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="44" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="46" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="48" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="50" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="52" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="54" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="56" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="58" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -595,7 +622,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G4" sqref="G4"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -759,13 +786,78 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="22.1640625" customWidth="1"/>
+    <col min="2" max="2" width="25.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="2">
+        <v>40000</v>
+      </c>
+      <c r="C2" s="1">
+        <v>43101</v>
+      </c>
+      <c r="D2" s="1">
+        <v>43190</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="2">
+        <v>60000</v>
+      </c>
+      <c r="C3" s="1">
+        <v>43191</v>
+      </c>
+      <c r="D3" s="1">
+        <v>43281</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="2">
+        <v>20000</v>
+      </c>
+      <c r="C4" s="1">
+        <v>43282</v>
+      </c>
+      <c r="D4" s="1">
+        <v>43373</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
ECP-949: moves project term from project to project item level
</commit_message>
<xml_diff>
--- a/estatioapp/app/src/test/java/org/estatio/module/capex/integtests/project/Projects OXF.xlsx
+++ b/estatioapp/app/src/test/java/org/estatio/module/capex/integtests/project/Projects OXF.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="33460" windowHeight="17900" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="35740" windowHeight="19040" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="projects" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="28">
   <si>
     <t>Project Reference</t>
   </si>
@@ -103,7 +103,7 @@
     <t>some works</t>
   </si>
   <si>
-    <t>budgetedAmount</t>
+    <t>Budgeted Amount</t>
   </si>
 </sst>
 </file>
@@ -162,9 +162,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="60">
+  <cellStyleXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -229,7 +241,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="60">
+  <cellStyles count="72">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
@@ -260,6 +272,12 @@
     <cellStyle name="Followed Hyperlink" xfId="55" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="57" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="59" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="61" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="63" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="65" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="67" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="69" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="71" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -289,6 +307,12 @@
     <cellStyle name="Hyperlink" xfId="54" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="56" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="58" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="60" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="62" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="64" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="66" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="68" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="70" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -622,7 +646,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomLeft" activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -786,72 +810,102 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="22.1640625" customWidth="1"/>
     <col min="2" max="2" width="25.6640625" customWidth="1"/>
+    <col min="3" max="3" width="19.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
         <v>27</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="2">
         <v>40000</v>
       </c>
-      <c r="C2" s="1">
+      <c r="D2" s="1">
         <v>43101</v>
       </c>
-      <c r="D2" s="1">
+      <c r="E2" s="1">
         <v>43190</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="2">
         <v>60000</v>
       </c>
-      <c r="C3" s="1">
+      <c r="D3" s="1">
         <v>43191</v>
       </c>
-      <c r="D3" s="1">
+      <c r="E3" s="1">
         <v>43281</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="2">
-        <v>20000</v>
-      </c>
-      <c r="C4" s="1">
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="2">
+        <v>5</v>
+      </c>
+      <c r="D4" s="1">
+        <v>43101</v>
+      </c>
+      <c r="E4" s="1">
+        <v>43190</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="2">
+        <v>15000</v>
+      </c>
+      <c r="D5" s="1">
         <v>43282</v>
       </c>
-      <c r="D4" s="1">
+      <c r="E5" s="1">
         <v>43373</v>
       </c>
     </row>

</xml_diff>